<commit_message>
Updated the report to the column names of the literature review
</commit_message>
<xml_diff>
--- a/LiteratureReviewResults.xlsx
+++ b/LiteratureReviewResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annekathrin/Documents/extrafiles/HIPSTER/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annekathrin/Documents/extrafiles/GSE130842_Showcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DF5899-456F-AB40-A940-D83D450AB327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB00535D-9EB8-E243-A36A-47BE4A269C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47420" yWindow="3660" windowWidth="30240" windowHeight="17140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32480" yWindow="3660" windowWidth="30240" windowHeight="17140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description of collected info" sheetId="1" r:id="rId1"/>
@@ -707,9 +707,6 @@
     <t>Metascape</t>
   </si>
   <si>
-    <t>IPA</t>
-  </si>
-  <si>
     <t>Not stated</t>
   </si>
   <si>
@@ -737,9 +734,6 @@
     <t>GSEA, gprofiler2</t>
   </si>
   <si>
-    <t>Panther, IPA</t>
-  </si>
-  <si>
     <t>Welch's t Test</t>
   </si>
   <si>
@@ -770,9 +764,6 @@
     <t>Network</t>
   </si>
   <si>
-    <t>Enrichment Map</t>
-  </si>
-  <si>
     <t>Violin Plot</t>
   </si>
   <si>
@@ -899,10 +890,6 @@
     <t>Enrichment Network</t>
   </si>
   <si>
-    <t>Enrichment Plot,Histogram,Scatter Plot
-IPA</t>
-  </si>
-  <si>
     <t>Venn Diagram</t>
   </si>
   <si>
@@ -1188,9 +1175,6 @@
     <t>Use of metascape to aggregate to 20 clusters</t>
   </si>
   <si>
-    <t>p value, biological relevance</t>
-  </si>
-  <si>
     <t>In order to remove redudancy, they did a further enrichment analysis with Revigo</t>
   </si>
   <si>
@@ -1222,6 +1206,21 @@
   </si>
   <si>
     <t>Scatter Plot, Histogram, Enrichment Plot</t>
+  </si>
+  <si>
+    <t>Panther, Inguenity Pathway Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inguenity Pathway Analysis</t>
+  </si>
+  <si>
+    <t>Enrichment Plot, Histogram, Scatter Plot</t>
+  </si>
+  <si>
+    <t>Heatmap, Enrichment Map</t>
+  </si>
+  <si>
+    <t>p value, Biological Relevance</t>
   </si>
 </sst>
 </file>
@@ -1504,10 +1503,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1770,18 +1765,18 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1794,7 +1789,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>208</v>
@@ -1802,7 +1797,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>209</v>
@@ -1810,7 +1805,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>210</v>
@@ -1818,7 +1813,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>211</v>
@@ -1842,10 +1837,10 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1861,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1967,7 +1962,7 @@
   </sheetPr>
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -2004,25 +1999,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>207</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>212</v>
@@ -2031,7 +2026,7 @@
         <v>214</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>4</v>
@@ -2057,19 +2052,19 @@
         <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I2" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K2" s="4" t="b">
         <v>0</v>
@@ -2081,13 +2076,13 @@
         <v>1</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2104,22 +2099,22 @@
         <v>145</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>135</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I3" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="K3" s="4" t="b">
         <v>0</v>
@@ -2134,10 +2129,10 @@
         <v>139</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2160,34 +2155,34 @@
         <v>32</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="M4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2207,19 +2202,19 @@
         <v>8</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I5" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K5" s="4" t="b">
         <v>0</v>
@@ -2234,10 +2229,10 @@
         <v>139</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2257,19 +2252,19 @@
         <v>8</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I6" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="K6" s="4" t="b">
         <v>0</v>
@@ -2284,10 +2279,10 @@
         <v>139</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2307,19 +2302,19 @@
         <v>217</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="K7" s="4" t="b">
         <v>0</v>
@@ -2334,7 +2329,7 @@
         <v>139</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P7" s="4" t="b">
         <v>1</v>
@@ -2360,16 +2355,16 @@
         <v>135</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="I8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K8" s="4" t="b">
         <v>0</v>
@@ -2381,13 +2376,13 @@
         <v>1</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2563,19 +2558,19 @@
         <v>8</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I12" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="K12" s="4" t="b">
         <v>0</v>
@@ -2590,10 +2585,10 @@
         <v>139</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2613,19 +2608,19 @@
         <v>8</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="I13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K13" s="4" t="b">
         <v>0</v>
@@ -2640,10 +2635,10 @@
         <v>139</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2663,19 +2658,19 @@
         <v>8</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I14" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="K14" s="4" t="b">
         <v>0</v>
@@ -2690,10 +2685,10 @@
         <v>139</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2710,22 +2705,22 @@
         <v>180</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I15" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="K15" s="4" t="b">
         <v>0</v>
@@ -2737,13 +2732,13 @@
         <v>1</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2766,16 +2761,16 @@
         <v>135</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="I16" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K16" s="4" t="b">
         <v>0</v>
@@ -2787,13 +2782,13 @@
         <v>1</v>
       </c>
       <c r="N16" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="O16" s="4" t="s">
-        <v>275</v>
-      </c>
       <c r="P16" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2813,19 +2808,19 @@
         <v>8</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I17" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K17" s="4" t="b">
         <v>0</v>
@@ -2837,13 +2832,13 @@
         <v>1</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2916,25 +2911,25 @@
         <v>8</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I19" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="K19" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="M19" s="4" t="b">
         <v>1</v>
@@ -2943,10 +2938,10 @@
         <v>139</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2966,19 +2961,19 @@
         <v>8</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I20" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K20" s="4" t="b">
         <v>0</v>
@@ -2990,13 +2985,13 @@
         <v>1</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3016,19 +3011,19 @@
         <v>8</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I21" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="K21" s="4" t="b">
         <v>0</v>
@@ -3040,13 +3035,13 @@
         <v>1</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3094,8 +3089,8 @@
   </sheetPr>
   <dimension ref="A1:AG1030"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3131,25 +3126,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>207</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>212</v>
@@ -3158,7 +3153,7 @@
         <v>214</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>4</v>
@@ -3195,7 +3190,7 @@
         <v>134</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>8</v>
@@ -3204,16 +3199,16 @@
         <v>135</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I2" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K2" s="4" t="b">
         <v>0</v>
@@ -3228,10 +3223,10 @@
         <v>139</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -3259,28 +3254,28 @@
         <v>102</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>220</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I3" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K3" s="4" t="b">
         <v>0</v>
@@ -3292,13 +3287,13 @@
         <v>1</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -3326,28 +3321,28 @@
         <v>103</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I4" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K4" s="4" t="b">
         <v>0</v>
@@ -3362,10 +3357,10 @@
         <v>139</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -3396,7 +3391,7 @@
         <v>136</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>218</v>
@@ -3460,10 +3455,10 @@
         <v>105</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>8</v>
@@ -3472,16 +3467,16 @@
         <v>29</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="I6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="K6" s="4" t="b">
         <v>0</v>
@@ -3493,13 +3488,13 @@
         <v>1</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -3527,28 +3522,28 @@
         <v>106</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K7" s="4" t="b">
         <v>0</v>
@@ -3563,10 +3558,10 @@
         <v>139</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -3594,28 +3589,28 @@
         <v>107</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K8" s="4" t="b">
         <v>0</v>
@@ -3627,13 +3622,13 @@
         <v>1</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -3661,10 +3656,10 @@
         <v>108</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>218</v>
@@ -3728,46 +3723,46 @@
         <v>109</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>287</v>
+        <v>392</v>
       </c>
       <c r="K10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="M10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -3795,28 +3790,28 @@
         <v>110</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I11" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="K11" s="4" t="b">
         <v>0</v>
@@ -3828,13 +3823,13 @@
         <v>1</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -3862,28 +3857,28 @@
         <v>111</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="I12" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K12" s="4" t="b">
         <v>0</v>
@@ -3895,13 +3890,13 @@
         <v>1</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
@@ -3929,46 +3924,46 @@
         <v>112</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="K13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="M13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
@@ -3996,10 +3991,10 @@
         <v>113</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>218</v>
@@ -4063,10 +4058,10 @@
         <v>114</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>218</v>
@@ -4130,10 +4125,10 @@
         <v>115</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>8</v>
@@ -4142,34 +4137,34 @@
         <v>220</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I16" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="K16" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="M16" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
@@ -4197,10 +4192,10 @@
         <v>116</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>218</v>
@@ -4264,10 +4259,10 @@
         <v>117</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>218</v>
@@ -4331,10 +4326,10 @@
         <v>118</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>218</v>
@@ -4398,10 +4393,10 @@
         <v>119</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>218</v>
@@ -4465,10 +4460,10 @@
         <v>120</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>218</v>
@@ -4532,19 +4527,19 @@
         <v>121</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>222</v>
@@ -4553,7 +4548,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="K22" s="4" t="b">
         <v>0</v>
@@ -4565,13 +4560,13 @@
         <v>1</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P22" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
@@ -4596,10 +4591,10 @@
         <v>122</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>8</v>
@@ -4608,34 +4603,34 @@
         <v>135</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I23" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K23" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="M23" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
@@ -4660,10 +4655,10 @@
         <v>123</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>218</v>
@@ -4730,25 +4725,25 @@
         <v>137</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I25" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="K25" s="4" t="b">
         <v>0</v>
@@ -4760,13 +4755,13 @@
         <v>1</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O25" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
@@ -4794,25 +4789,25 @@
         <v>138</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>217</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="I26" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="K26" s="4" t="b">
         <v>0</v>
@@ -4824,13 +4819,13 @@
         <v>1</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
@@ -4855,10 +4850,10 @@
         <v>126</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>8</v>
@@ -4867,34 +4862,34 @@
         <v>29</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I27" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K27" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="M27" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O27" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
@@ -4919,10 +4914,10 @@
         <v>127</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>218</v>
@@ -4986,10 +4981,10 @@
         <v>128</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>218</v>
@@ -5053,10 +5048,10 @@
         <v>129</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>217</v>
@@ -5065,16 +5060,16 @@
         <v>219</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I30" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K30" s="4" t="b">
         <v>0</v>
@@ -5086,13 +5081,13 @@
         <v>1</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
@@ -5117,28 +5112,28 @@
         <v>130</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I31" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="K31" s="4" t="b">
         <v>0</v>
@@ -5150,13 +5145,13 @@
         <v>1</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5167,10 +5162,10 @@
         <v>131</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>218</v>
@@ -5234,19 +5229,19 @@
         <v>132</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>222</v>
@@ -5255,25 +5250,25 @@
         <v>1</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="K33" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="M33" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O33" s="14" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
@@ -5298,10 +5293,10 @@
         <v>133</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>8</v>
@@ -5310,16 +5305,16 @@
         <v>220</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I34" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K34" s="4" t="b">
         <v>0</v>
@@ -5331,13 +5326,13 @@
         <v>1</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -36253,8 +36248,8 @@
   </sheetPr>
   <dimension ref="A1:Y45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -36282,25 +36277,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>207</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>212</v>
@@ -36309,7 +36304,7 @@
         <v>214</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>4</v>
@@ -36335,7 +36330,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>221</v>
@@ -36347,13 +36342,13 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="K2" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="M2" s="4" t="b">
         <v>1</v>
@@ -36362,7 +36357,7 @@
         <v>139</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="P2" s="4" t="b">
         <v>1</v>
@@ -36385,19 +36380,19 @@
         <v>8</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>221</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>223</v>
+        <v>391</v>
       </c>
       <c r="I3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="K3" s="4" t="b">
         <v>0</v>
@@ -36409,13 +36404,13 @@
         <v>1</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -36435,19 +36430,19 @@
         <v>8</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I4" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="K4" s="4" t="b">
         <v>0</v>
@@ -36459,10 +36454,10 @@
         <v>1</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P4" s="4" t="b">
         <v>1</v>
@@ -36488,16 +36483,16 @@
         <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>226</v>
       </c>
       <c r="I5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K5" s="4" t="b">
         <v>0</v>
@@ -36509,10 +36504,10 @@
         <v>1</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P5" s="4" t="b">
         <v>1</v>
@@ -36715,16 +36710,16 @@
         <v>219</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>228</v>
       </c>
       <c r="I9" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K9" s="4" t="b">
         <v>0</v>
@@ -36736,10 +36731,10 @@
         <v>1</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P9" s="4" t="b">
         <v>1</v>
@@ -36824,7 +36819,7 @@
         <v>29</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>222</v>
@@ -36833,7 +36828,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="K11" s="4" t="b">
         <v>0</v>
@@ -36845,13 +36840,13 @@
         <v>1</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -36877,13 +36872,13 @@
         <v>221</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I12" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K12" s="4" t="b">
         <v>0</v>
@@ -36895,13 +36890,13 @@
         <v>1</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -36924,16 +36919,16 @@
         <v>29</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K13" s="4" t="b">
         <v>0</v>
@@ -36945,10 +36940,10 @@
         <v>1</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="P13" s="4" t="b">
         <v>1</v>
@@ -37089,19 +37084,19 @@
         <v>8</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I16" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K16" s="4" t="b">
         <v>0</v>
@@ -37113,13 +37108,13 @@
         <v>1</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -37378,16 +37373,16 @@
         <v>29</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I21" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K21" s="4" t="b">
         <v>0</v>
@@ -37399,10 +37394,10 @@
         <v>1</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="P21" s="4" t="b">
         <v>1</v>
@@ -37602,19 +37597,19 @@
         <v>8</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I25" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K25" s="4" t="b">
         <v>0</v>
@@ -37626,13 +37621,13 @@
         <v>1</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -37655,31 +37650,31 @@
         <v>29</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I26" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K26" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="M26" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="P26" s="4" t="b">
         <v>1</v>
@@ -37702,19 +37697,19 @@
         <v>217</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="I27" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K27" s="4" t="b">
         <v>0</v>
@@ -37726,10 +37721,10 @@
         <v>1</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P27" s="4" t="b">
         <v>1</v>
@@ -37755,16 +37750,16 @@
         <v>220</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I28" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K28" s="4" t="b">
         <v>0</v>
@@ -37776,10 +37771,10 @@
         <v>1</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P28" s="4" t="b">
         <v>1</v>
@@ -37802,37 +37797,37 @@
         <v>217</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I29" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="K29" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M29" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -37914,16 +37909,16 @@
         <v>29</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>233</v>
+        <v>390</v>
       </c>
       <c r="I31" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K31" s="4" t="b">
         <v>0</v>
@@ -37935,13 +37930,13 @@
         <v>1</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -37964,16 +37959,16 @@
         <v>29</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I32" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K32" s="4" t="b">
         <v>0</v>
@@ -37985,10 +37980,10 @@
         <v>1</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P32" s="4" t="b">
         <v>1</v>
@@ -38309,31 +38304,31 @@
         <v>29</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I38" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K38" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M38" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="O38" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P38" s="4" t="b">
         <v>1</v>
@@ -38536,31 +38531,31 @@
         <v>29</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I42" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="K42" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M42" s="4" t="b">
         <v>1</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P42" s="4" t="b">
         <v>1</v>
@@ -38586,16 +38581,16 @@
         <v>96</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I43" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K43" s="4" t="b">
         <v>0</v>
@@ -38607,10 +38602,10 @@
         <v>1</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P43" s="4" t="b">
         <v>1</v>

</xml_diff>